<commit_message>
Making a lot of progress!
</commit_message>
<xml_diff>
--- a/User-TEST.xlsx
+++ b/User-TEST.xlsx
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,97 +579,59 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="4">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3">
-        <v>28755</v>
-      </c>
-      <c r="H3" s="4">
-        <v>90</v>
-      </c>
-      <c r="I3" s="4">
-        <v>198</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3">
-        <v>31575</v>
+        <v>28755</v>
       </c>
       <c r="H4" s="4">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="I4" s="4">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
@@ -695,49 +657,87 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3">
+        <v>31575</v>
+      </c>
+      <c r="H6" s="4">
+        <v>110</v>
+      </c>
+      <c r="I6" s="4">
+        <v>205</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E7" s="4">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G7" s="3">
         <v>28755</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H7" s="4">
         <v>90</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I7" s="4">
         <v>198</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>23</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>37</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L7" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Working OK. Cleaning UP and tweaking a bit - enhancement.
</commit_message>
<xml_diff>
--- a/User-TEST.xlsx
+++ b/User-TEST.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="49">
   <si>
     <t>EMAIL_ADDRESS</t>
   </si>
@@ -131,6 +131,36 @@
   </si>
   <si>
     <t>as</t>
+  </si>
+  <si>
+    <t>dsjhds1@fdkfjdk.com</t>
+  </si>
+  <si>
+    <t>luka.doncic1@me.com</t>
+  </si>
+  <si>
+    <t>ian.intermediate1@gmail.com</t>
+  </si>
+  <si>
+    <t>nick.newbie1@gmail.com</t>
+  </si>
+  <si>
+    <t>dsjhds2@fdkfjdk.com</t>
+  </si>
+  <si>
+    <t>luka.doncic2@me.com</t>
+  </si>
+  <si>
+    <t>ian.intermediate2@gmail.com</t>
+  </si>
+  <si>
+    <t>nick.newbie2@gmail.com</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -492,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,6 +761,310 @@
         <v>31</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3">
+        <v>28755</v>
+      </c>
+      <c r="H8" s="4">
+        <v>90</v>
+      </c>
+      <c r="I8" s="4">
+        <v>198</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3">
+        <v>31575</v>
+      </c>
+      <c r="H9" s="4">
+        <v>110</v>
+      </c>
+      <c r="I9" s="4">
+        <v>205</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3">
+        <v>31575</v>
+      </c>
+      <c r="H10" s="4">
+        <v>110</v>
+      </c>
+      <c r="I10" s="4">
+        <v>205</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="3">
+        <v>28755</v>
+      </c>
+      <c r="H11" s="4">
+        <v>90</v>
+      </c>
+      <c r="I11" s="4">
+        <v>198</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3">
+        <v>28755</v>
+      </c>
+      <c r="H12" s="4">
+        <v>90</v>
+      </c>
+      <c r="I12" s="4">
+        <v>198</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="4">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="3">
+        <v>31575</v>
+      </c>
+      <c r="H13" s="4">
+        <v>110</v>
+      </c>
+      <c r="I13" s="4">
+        <v>205</v>
+      </c>
+      <c r="J13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3">
+        <v>31575</v>
+      </c>
+      <c r="H14" s="4">
+        <v>110</v>
+      </c>
+      <c r="I14" s="4">
+        <v>205</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="3">
+        <v>28755</v>
+      </c>
+      <c r="H15" s="4">
+        <v>90</v>
+      </c>
+      <c r="I15" s="4">
+        <v>198</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
@@ -738,8 +1072,16 @@
     <hyperlink ref="C5" r:id="rId3"/>
     <hyperlink ref="C6" r:id="rId4"/>
     <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C10" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId9"/>
+    <hyperlink ref="C12" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
+    <hyperlink ref="C14" r:id="rId12"/>
+    <hyperlink ref="C15" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>